<commit_message>
implement basic unit test
</commit_message>
<xml_diff>
--- a/data/MONTE_CARLO_ASSUMPTIONS.xlsx
+++ b/data/MONTE_CARLO_ASSUMPTIONS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geyerbisschoff\PythonProjects\Z-model\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\users\geyerbisschoff\pythonprojects\z-model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1274960B-AF2A-4683-A448-2E5520CB5B2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A65336-EFFB-4816-9F4F-85CC9D174766}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="-120" windowWidth="27645" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40212" yWindow="-6528" windowWidth="40320" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DATA" sheetId="1" r:id="rId1"/>
@@ -1328,7 +1328,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="K2" sqref="K2:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1415,7 +1415,7 @@
         <v>2.41E-2</v>
       </c>
       <c r="K2" s="14">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="L2" s="14" t="s">
         <v>13</v>
@@ -1455,7 +1455,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="14">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="L3" s="14"/>
     </row>
@@ -1493,7 +1493,7 @@
         <v>0.42899999999999999</v>
       </c>
       <c r="K4" s="14">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="L4" s="14"/>
     </row>
@@ -1531,7 +1531,7 @@
         <v>0.42899999999999999</v>
       </c>
       <c r="K5" s="14">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="L5" s="14"/>
     </row>

</xml_diff>